<commit_message>
tweaking test version to print paths, dont move anything
</commit_message>
<xml_diff>
--- a/HerbariumHours.xlsx
+++ b/HerbariumHours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,10 +49,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,14 +91,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,7 +435,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -471,12 +491,20 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="G3">
+        <f>SUM(B3:F3)</f>
+        <v>2.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="A2:A3" twoDigitTextYear="1"/>
-    <ignoredError sqref="G2" emptyCellReference="1"/>
+    <ignoredError sqref="G2:G3" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
gui pseudocode & openrefine fix
</commit_message>
<xml_diff>
--- a/HerbariumHours.xlsx
+++ b/HerbariumHours.xlsx
@@ -457,7 +457,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f>SUM(B2:F2)</f>
+        <f t="shared" ref="G2:G7" si="0">SUM(B2:F2)</f>
         <v>9.5</v>
       </c>
     </row>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>SUM(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -553,7 +553,7 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f>SUM(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <f>SUM(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -601,7 +601,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>SUM(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -625,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="G7">
-        <f>SUM(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -634,7 +634,16 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>3.5</v>
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replacing blank with X, then with unspecified
</commit_message>
<xml_diff>
--- a/HerbariumHours.xlsx
+++ b/HerbariumHours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="500" windowWidth="25040" windowHeight="14040" tabRatio="500"/>
+    <workbookView xWindow="29340" yWindow="-20" windowWidth="25040" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Monday</t>
   </si>
@@ -60,7 +60,10 @@
     <t>9/24-28</t>
   </si>
   <si>
-    <t>10/1-8</t>
+    <t>10/8-12</t>
+  </si>
+  <si>
+    <t>10/1-4</t>
   </si>
 </sst>
 </file>
@@ -454,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -505,7 +508,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G7" si="0">SUM(B2:F2)</f>
+        <f t="shared" ref="G2:G8" si="0">SUM(B2:F2)</f>
         <v>9.5</v>
       </c>
     </row>
@@ -631,7 +634,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -644,6 +647,21 @@
       </c>
       <c r="E8">
         <v>2.5</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mostly working on reorganizing script
</commit_message>
<xml_diff>
--- a/HerbariumHours.xlsx
+++ b/HerbariumHours.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Monday</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>10/15-19</t>
+  </si>
+  <si>
+    <t>10/22-26</t>
+  </si>
+  <si>
+    <t>10/29-11/2</t>
   </si>
 </sst>
 </file>
@@ -115,8 +121,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -128,13 +140,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -515,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G9" si="0">SUM(B2:F2)</f>
+        <f t="shared" ref="G2:G12" si="0">SUM(B2:F2)</f>
         <v>9.5</v>
       </c>
     </row>
@@ -696,6 +714,64 @@
       </c>
       <c r="C10">
         <v>1.5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>